<commit_message>
Solved Native PDF Read type String
</commit_message>
<xml_diff>
--- a/EmploymentProcess/ExcelDataTables/Applicants.xlsx
+++ b/EmploymentProcess/ExcelDataTables/Applicants.xlsx
@@ -1,72 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <x:bookViews>
-    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="0" activeTab="0"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="122211"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="122211"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t xml:space="preserve"> Technical College / High School – Miodrag Belodedici of Brașov</t>
+  </si>
+  <si>
+    <t>Bobocel Murgulescu_x000D_</t>
+  </si>
+  <si>
+    <t>bobom@fictivemail.ro_x000D_</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-</x:styleSheet>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -112,7 +120,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -147,7 +155,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,26 +363,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:5">
-      <x:c r="A1" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>407092783</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>